<commit_message>
save tidy dataset as Excel file
</commit_message>
<xml_diff>
--- a/inst/extdata/Artificial Lift Matrix for Commercial Production Systems (CPS)14Aug062.xlsx
+++ b/inst/extdata/Artificial Lift Matrix for Commercial Production Systems (CPS)14Aug062.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\github-oilgains\artificial_lift_matrix\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FD6870-6497-47FD-984C-7737E71614C0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB52BAF7-18A7-451A-8F04-50A07DA18C01}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="15" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,14 @@
   </sheets>
   <definedNames>
     <definedName name="OLE_LINK4" localSheetId="0">'Artificial Lift Matrix'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Artificial Lift Matrix'!$A$1:$S$70</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Artificial Lift Matrix'!$A$1:$S$77</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="112">
   <si>
     <t xml:space="preserve"> Design Aspect</t>
   </si>
@@ -128,12 +128,6 @@
     <t>Dogleg Severity</t>
   </si>
   <si>
-    <t>&lt; 3 º/100’</t>
-  </si>
-  <si>
-    <t>&gt; 10 º/100’</t>
-  </si>
-  <si>
     <t>Safety Barriers</t>
   </si>
   <si>
@@ -278,9 +272,6 @@
     <t>Lo Surf Leak Risk</t>
   </si>
   <si>
-    <t>Operating cost (low)</t>
-  </si>
-  <si>
     <t>Relative Intervention Frequency</t>
   </si>
   <si>
@@ -320,11 +311,44 @@
     <t>Fluid viscosity (cp)</t>
   </si>
   <si>
-    <t>9.625” &amp; larger</t>
+    <t>&lt; 1.5 per Well/yr</t>
+  </si>
+  <si>
+    <t>Operating Temp (degF)</t>
+  </si>
+  <si>
+    <t>250-500</t>
+  </si>
+  <si>
+    <t>100-250</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Metal PCP (Hi Temp)</t>
+  </si>
+  <si>
+    <t>ESP-CP</t>
+  </si>
+  <si>
+    <t>Sucker Rod Pump</t>
+  </si>
+  <si>
+    <t>9.625" and larger</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Operating cost</t>
+  </si>
+  <si>
+    <t>&lt; 3 deg / 100'</t>
   </si>
   <si>
     <r>
-      <t>3 - 10</t>
+      <t>3 - 10 deg</t>
     </r>
     <r>
       <rPr>
@@ -334,7 +358,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">º </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -347,28 +371,16 @@
     </r>
   </si>
   <si>
-    <t>&lt; 1.5 per Well/yr</t>
-  </si>
-  <si>
-    <t>Operating Temp (degF)</t>
-  </si>
-  <si>
-    <t>250-500</t>
-  </si>
-  <si>
-    <t>100-250</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Metal PCP (Hi Temp)</t>
-  </si>
-  <si>
-    <t>ESP-CP</t>
-  </si>
-  <si>
-    <t>Sucker Rod Pump</t>
+    <t>&gt; 10 deg / 100'</t>
+  </si>
+  <si>
+    <t>Operating Cost</t>
+  </si>
+  <si>
+    <t>Setup cost</t>
+  </si>
+  <si>
+    <t>small</t>
   </si>
 </sst>
 </file>
@@ -861,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1093,6 +1105,27 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1496,10 +1529,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AL91"/>
+  <dimension ref="A1:AL98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <pane xSplit="3240" ySplit="1890" topLeftCell="A54" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
+      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1507,7 +1543,7 @@
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" customWidth="1"/>
     <col min="3" max="3" width="33.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
     <col min="16" max="16" width="11.85546875" customWidth="1"/>
     <col min="17" max="18" width="11.85546875" hidden="1" customWidth="1"/>
     <col min="19" max="22" width="4.7109375" customWidth="1"/>
@@ -1582,7 +1618,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1645,7 +1681,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E5" s="40" t="s">
         <v>1</v>
@@ -1657,16 +1693,16 @@
         <v>3</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="I5" s="40" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="40" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K5" s="40" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L5" s="40" t="s">
         <v>5</v>
@@ -1950,7 +1986,7 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="77" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D10" s="66" t="s">
         <v>19</v>
@@ -2012,7 +2048,7 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="77" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D11" s="67" t="s">
         <v>21</v>
@@ -2072,7 +2108,7 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="77" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D12" s="67" t="s">
         <v>22</v>
@@ -2252,7 +2288,7 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="63" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D15" s="69" t="s">
         <v>17</v>
@@ -2312,10 +2348,10 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="63" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D16" s="70" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E16" s="10">
         <v>2</v>
@@ -2372,10 +2408,10 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="63" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D17" s="71" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E17" s="9">
         <v>3</v>
@@ -2495,7 +2531,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="71" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E19" s="24">
         <v>2</v>
@@ -2738,7 +2774,7 @@
         <v>33</v>
       </c>
       <c r="D23" s="66" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="E23" s="16">
         <v>3</v>
@@ -2798,7 +2834,7 @@
         <v>33</v>
       </c>
       <c r="D24" s="67" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E24" s="9">
         <v>3</v>
@@ -2858,7 +2894,7 @@
         <v>33</v>
       </c>
       <c r="D25" s="72" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
       <c r="E25" s="11">
         <v>3</v>
@@ -2915,10 +2951,10 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="78" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D26" s="73" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E26" s="22">
         <v>1</v>
@@ -2975,10 +3011,10 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="77" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D27" s="66" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E27" s="16">
         <v>3</v>
@@ -3035,10 +3071,10 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="77" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D28" s="71" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E28" s="11">
         <v>3</v>
@@ -3095,10 +3131,10 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="77" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="66" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E29" s="27">
         <v>1</v>
@@ -3155,10 +3191,10 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="77" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D30" s="66" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E30" s="16">
         <v>3</v>
@@ -3215,10 +3251,10 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="77" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="71" t="s">
         <v>42</v>
-      </c>
-      <c r="D31" s="71" t="s">
-        <v>44</v>
       </c>
       <c r="E31" s="20">
         <v>1</v>
@@ -3275,10 +3311,10 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="63" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D32" s="71" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E32" s="16">
         <v>3</v>
@@ -3335,10 +3371,10 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="77" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D33" s="66" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E33" s="16">
         <v>3</v>
@@ -3395,10 +3431,10 @@
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="71" t="s">
         <v>47</v>
-      </c>
-      <c r="D34" s="71" t="s">
-        <v>49</v>
       </c>
       <c r="E34" s="24">
         <v>2</v>
@@ -3455,10 +3491,10 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="77" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D35" s="66" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E35" s="18">
         <v>2</v>
@@ -3515,10 +3551,10 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="67" t="s">
         <v>50</v>
-      </c>
-      <c r="D36" s="67" t="s">
-        <v>52</v>
       </c>
       <c r="E36" s="9">
         <v>3</v>
@@ -3575,10 +3611,10 @@
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="77" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D37" s="71" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E37" s="11">
         <v>3</v>
@@ -3635,10 +3671,10 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="77" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D38" s="66" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E38" s="16">
         <v>3</v>
@@ -3695,10 +3731,10 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="77" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D39" s="67" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E39" s="9">
         <v>3</v>
@@ -3755,10 +3791,10 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="77" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D40" s="71" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E40" s="24">
         <v>2</v>
@@ -3815,10 +3851,10 @@
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="77" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D41" s="66" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E41" s="16">
         <v>3</v>
@@ -3875,11 +3911,11 @@
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="77" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="67" t="s">
-        <v>59</v>
-      </c>
       <c r="E42" s="10">
         <v>2</v>
       </c>
@@ -3905,7 +3941,7 @@
         <v>2</v>
       </c>
       <c r="M42" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N42" s="12">
         <v>3</v>
@@ -3935,10 +3971,10 @@
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="77" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D43" s="71" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E43" s="20">
         <v>1</v>
@@ -3965,7 +4001,7 @@
         <v>2</v>
       </c>
       <c r="M43" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="N43" s="25">
         <v>2</v>
@@ -3995,10 +4031,10 @@
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="77" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D44" s="66" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E44" s="16">
         <v>3</v>
@@ -4055,10 +4091,10 @@
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="67" t="s">
         <v>62</v>
-      </c>
-      <c r="D45" s="67" t="s">
-        <v>64</v>
       </c>
       <c r="E45" s="10">
         <v>2</v>
@@ -4115,10 +4151,10 @@
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="77" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D46" s="71" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E46" s="24">
         <v>2</v>
@@ -4171,14 +4207,14 @@
       <c r="AD46" s="1"/>
       <c r="AL46" s="1"/>
     </row>
-    <row r="47" spans="1:38" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="64" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D47" s="74" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E47" s="10">
         <v>2</v>
@@ -4235,10 +4271,10 @@
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="77" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D48" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E48" s="18">
         <v>2</v>
@@ -4295,10 +4331,10 @@
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="D49" s="67" t="s">
         <v>68</v>
-      </c>
-      <c r="D49" s="67" t="s">
-        <v>70</v>
       </c>
       <c r="E49" s="10">
         <v>2</v>
@@ -4355,10 +4391,10 @@
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="77" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D50" s="67" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E50" s="10">
         <v>2</v>
@@ -4415,10 +4451,10 @@
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="77" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D51" s="71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E51" s="24">
         <v>2</v>
@@ -4475,10 +4511,10 @@
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="77" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D52" s="66" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E52" s="16">
         <v>3</v>
@@ -4535,10 +4571,10 @@
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="71" t="s">
         <v>73</v>
-      </c>
-      <c r="D53" s="71" t="s">
-        <v>75</v>
       </c>
       <c r="E53" s="11">
         <v>3</v>
@@ -4595,10 +4631,10 @@
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="77" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D54" s="66" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E54" s="16">
         <v>3</v>
@@ -4655,10 +4691,10 @@
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="77" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="67" t="s">
         <v>76</v>
-      </c>
-      <c r="D55" s="67" t="s">
-        <v>78</v>
       </c>
       <c r="E55" s="9">
         <v>3</v>
@@ -4715,10 +4751,10 @@
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="77" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D56" s="67" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E56" s="9">
         <v>3</v>
@@ -4775,10 +4811,10 @@
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="77" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D57" s="71" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E57" s="11">
         <v>3</v>
@@ -4835,10 +4871,10 @@
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="77" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D58" s="66" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E58" s="16">
         <v>3</v>
@@ -4897,10 +4933,10 @@
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="D59" s="71" t="s">
         <v>81</v>
-      </c>
-      <c r="D59" s="71" t="s">
-        <v>83</v>
       </c>
       <c r="E59" s="24">
         <v>2</v>
@@ -4959,9 +4995,11 @@
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="77" t="s">
-        <v>84</v>
-      </c>
-      <c r="D60" s="75"/>
+        <v>105</v>
+      </c>
+      <c r="D60" s="75" t="s">
+        <v>104</v>
+      </c>
       <c r="E60" s="10">
         <v>2</v>
       </c>
@@ -5017,10 +5055,10 @@
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="65" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D61" s="76" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E61" s="55">
         <v>3</v>
@@ -5073,25 +5111,53 @@
       <c r="AD61" s="1"/>
       <c r="AL61" s="1"/>
     </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:38" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
+      <c r="C62" s="82" t="s">
+        <v>110</v>
+      </c>
+      <c r="D62" s="83" t="s">
+        <v>111</v>
+      </c>
+      <c r="E62" s="84">
+        <v>1</v>
+      </c>
+      <c r="F62" s="85">
+        <v>1</v>
+      </c>
+      <c r="G62" s="84">
+        <v>2</v>
+      </c>
+      <c r="H62" s="84">
+        <v>3</v>
+      </c>
+      <c r="I62" s="86">
+        <v>3</v>
+      </c>
+      <c r="J62" s="85">
+        <v>2</v>
+      </c>
+      <c r="K62" s="85">
+        <v>3</v>
+      </c>
+      <c r="L62" s="87">
+        <v>1</v>
+      </c>
+      <c r="M62" s="86">
+        <v>1</v>
+      </c>
+      <c r="N62" s="86">
+        <v>1</v>
+      </c>
+      <c r="O62" s="85">
+        <v>1</v>
+      </c>
+      <c r="P62" s="84">
+        <v>2</v>
+      </c>
+      <c r="Q62" s="88"/>
+      <c r="R62" s="88"/>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
@@ -5100,28 +5166,58 @@
       <c r="X62" s="1"/>
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
+      <c r="AB62" s="1"/>
+      <c r="AC62" s="1"/>
+      <c r="AD62" s="1"/>
       <c r="AL62" s="1"/>
     </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:38" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
-      <c r="B63" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63" s="83" t="s">
+        <v>111</v>
+      </c>
+      <c r="E63" s="84">
+        <v>1</v>
+      </c>
+      <c r="F63" s="85">
+        <v>2</v>
+      </c>
+      <c r="G63" s="84">
+        <v>3</v>
+      </c>
+      <c r="H63" s="84">
+        <v>1</v>
+      </c>
+      <c r="I63" s="86">
+        <v>1</v>
+      </c>
+      <c r="J63" s="85">
+        <v>1</v>
+      </c>
+      <c r="K63" s="85">
+        <v>1</v>
+      </c>
+      <c r="L63" s="87">
+        <v>2</v>
+      </c>
+      <c r="M63" s="86">
+        <v>2</v>
+      </c>
+      <c r="N63" s="86">
+        <v>1</v>
+      </c>
+      <c r="O63" s="85">
+        <v>1</v>
+      </c>
+      <c r="P63" s="84">
+        <v>2</v>
+      </c>
+      <c r="Q63" s="88"/>
+      <c r="R63" s="88"/>
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
@@ -5130,27 +5226,30 @@
       <c r="X63" s="1"/>
       <c r="Y63" s="1"/>
       <c r="Z63" s="1"/>
+      <c r="AB63" s="1"/>
+      <c r="AC63" s="1"/>
+      <c r="AD63" s="1"/>
       <c r="AL63" s="1"/>
     </row>
-    <row r="64" spans="1:38" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:38" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
-      <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
+      <c r="C64" s="82"/>
+      <c r="D64" s="83"/>
+      <c r="E64" s="84"/>
+      <c r="F64" s="85"/>
+      <c r="G64" s="84"/>
+      <c r="H64" s="84"/>
+      <c r="I64" s="86"/>
+      <c r="J64" s="85"/>
+      <c r="K64" s="85"/>
+      <c r="L64" s="87"/>
+      <c r="M64" s="86"/>
+      <c r="N64" s="86"/>
+      <c r="O64" s="85"/>
+      <c r="P64" s="84"/>
+      <c r="Q64" s="88"/>
+      <c r="R64" s="88"/>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
@@ -5159,31 +5258,30 @@
       <c r="X64" s="1"/>
       <c r="Y64" s="1"/>
       <c r="Z64" s="1"/>
+      <c r="AB64" s="1"/>
+      <c r="AC64" s="1"/>
+      <c r="AD64" s="1"/>
       <c r="AL64" s="1"/>
     </row>
-    <row r="65" spans="1:38" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:38" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
-      <c r="B65" s="4">
-        <v>3</v>
-      </c>
-      <c r="C65" s="79" t="s">
-        <v>87</v>
-      </c>
-      <c r="D65" s="80"/>
-      <c r="E65" s="80"/>
-      <c r="F65" s="80"/>
-      <c r="G65" s="80"/>
-      <c r="H65" s="80"/>
-      <c r="I65" s="80"/>
-      <c r="J65" s="80"/>
-      <c r="K65" s="80"/>
-      <c r="L65" s="80"/>
-      <c r="M65" s="81"/>
-      <c r="N65" s="54"/>
-      <c r="O65" s="54"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="82"/>
+      <c r="D65" s="83"/>
+      <c r="E65" s="84"/>
+      <c r="F65" s="85"/>
+      <c r="G65" s="84"/>
+      <c r="H65" s="84"/>
+      <c r="I65" s="86"/>
+      <c r="J65" s="85"/>
+      <c r="K65" s="85"/>
+      <c r="L65" s="87"/>
+      <c r="M65" s="86"/>
+      <c r="N65" s="86"/>
+      <c r="O65" s="85"/>
+      <c r="P65" s="84"/>
+      <c r="Q65" s="88"/>
+      <c r="R65" s="88"/>
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
@@ -5192,31 +5290,30 @@
       <c r="X65" s="1"/>
       <c r="Y65" s="1"/>
       <c r="Z65" s="1"/>
+      <c r="AB65" s="1"/>
+      <c r="AC65" s="1"/>
+      <c r="AD65" s="1"/>
       <c r="AL65" s="1"/>
     </row>
-    <row r="66" spans="1:38" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:38" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
-      <c r="B66" s="5">
-        <v>2</v>
-      </c>
-      <c r="C66" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="D66" s="80"/>
-      <c r="E66" s="80"/>
-      <c r="F66" s="80"/>
-      <c r="G66" s="80"/>
-      <c r="H66" s="80"/>
-      <c r="I66" s="80"/>
-      <c r="J66" s="80"/>
-      <c r="K66" s="80"/>
-      <c r="L66" s="80"/>
-      <c r="M66" s="81"/>
-      <c r="N66" s="54"/>
-      <c r="O66" s="54"/>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="82"/>
+      <c r="D66" s="83"/>
+      <c r="E66" s="84"/>
+      <c r="F66" s="85"/>
+      <c r="G66" s="84"/>
+      <c r="H66" s="84"/>
+      <c r="I66" s="86"/>
+      <c r="J66" s="85"/>
+      <c r="K66" s="85"/>
+      <c r="L66" s="87"/>
+      <c r="M66" s="86"/>
+      <c r="N66" s="86"/>
+      <c r="O66" s="85"/>
+      <c r="P66" s="84"/>
+      <c r="Q66" s="88"/>
+      <c r="R66" s="88"/>
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
@@ -5225,31 +5322,30 @@
       <c r="X66" s="1"/>
       <c r="Y66" s="1"/>
       <c r="Z66" s="1"/>
+      <c r="AB66" s="1"/>
+      <c r="AC66" s="1"/>
+      <c r="AD66" s="1"/>
       <c r="AL66" s="1"/>
     </row>
-    <row r="67" spans="1:38" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:38" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
-      <c r="B67" s="6">
-        <v>1</v>
-      </c>
-      <c r="C67" s="79" t="s">
-        <v>89</v>
-      </c>
-      <c r="D67" s="80"/>
-      <c r="E67" s="80"/>
-      <c r="F67" s="80"/>
-      <c r="G67" s="80"/>
-      <c r="H67" s="80"/>
-      <c r="I67" s="80"/>
-      <c r="J67" s="80"/>
-      <c r="K67" s="80"/>
-      <c r="L67" s="80"/>
-      <c r="M67" s="81"/>
-      <c r="N67" s="54"/>
-      <c r="O67" s="54"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="82"/>
+      <c r="D67" s="83"/>
+      <c r="E67" s="84"/>
+      <c r="F67" s="85"/>
+      <c r="G67" s="84"/>
+      <c r="H67" s="84"/>
+      <c r="I67" s="86"/>
+      <c r="J67" s="85"/>
+      <c r="K67" s="85"/>
+      <c r="L67" s="87"/>
+      <c r="M67" s="86"/>
+      <c r="N67" s="86"/>
+      <c r="O67" s="85"/>
+      <c r="P67" s="84"/>
+      <c r="Q67" s="88"/>
+      <c r="R67" s="88"/>
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
@@ -5258,31 +5354,30 @@
       <c r="X67" s="1"/>
       <c r="Y67" s="1"/>
       <c r="Z67" s="1"/>
+      <c r="AB67" s="1"/>
+      <c r="AC67" s="1"/>
+      <c r="AD67" s="1"/>
       <c r="AL67" s="1"/>
     </row>
-    <row r="68" spans="1:38" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:38" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
-      <c r="B68" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C68" s="79" t="s">
-        <v>91</v>
-      </c>
-      <c r="D68" s="80"/>
-      <c r="E68" s="80"/>
-      <c r="F68" s="80"/>
-      <c r="G68" s="80"/>
-      <c r="H68" s="80"/>
-      <c r="I68" s="80"/>
-      <c r="J68" s="80"/>
-      <c r="K68" s="80"/>
-      <c r="L68" s="80"/>
-      <c r="M68" s="81"/>
-      <c r="N68" s="54"/>
-      <c r="O68" s="54"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="82"/>
+      <c r="D68" s="83"/>
+      <c r="E68" s="84"/>
+      <c r="F68" s="85"/>
+      <c r="G68" s="84"/>
+      <c r="H68" s="84"/>
+      <c r="I68" s="86"/>
+      <c r="J68" s="85"/>
+      <c r="K68" s="85"/>
+      <c r="L68" s="87"/>
+      <c r="M68" s="86"/>
+      <c r="N68" s="86"/>
+      <c r="O68" s="85"/>
+      <c r="P68" s="84"/>
+      <c r="Q68" s="88"/>
+      <c r="R68" s="88"/>
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
@@ -5291,12 +5386,15 @@
       <c r="X68" s="1"/>
       <c r="Y68" s="1"/>
       <c r="Z68" s="1"/>
+      <c r="AB68" s="1"/>
+      <c r="AC68" s="1"/>
+      <c r="AD68" s="1"/>
       <c r="AL68" s="1"/>
     </row>
     <row r="69" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="C69" s="3"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -5322,11 +5420,10 @@
       <c r="Z69" s="1"/>
       <c r="AL69" s="1"/>
     </row>
-    <row r="70" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1" t="s">
-        <v>92</v>
+      <c r="B70" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -5353,12 +5450,10 @@
       <c r="Z70" s="1"/>
       <c r="AL70" s="1"/>
     </row>
-    <row r="71" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:38" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
-      <c r="C71" s="53" t="s">
-        <v>93</v>
-      </c>
+      <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -5384,22 +5479,26 @@
       <c r="Z71" s="1"/>
       <c r="AL71" s="1"/>
     </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:38" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
+      <c r="B72" s="4">
+        <v>3</v>
+      </c>
+      <c r="C72" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="D72" s="80"/>
+      <c r="E72" s="80"/>
+      <c r="F72" s="80"/>
+      <c r="G72" s="80"/>
+      <c r="H72" s="80"/>
+      <c r="I72" s="80"/>
+      <c r="J72" s="80"/>
+      <c r="K72" s="80"/>
+      <c r="L72" s="80"/>
+      <c r="M72" s="81"/>
+      <c r="N72" s="54"/>
+      <c r="O72" s="54"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
@@ -5413,22 +5512,26 @@
       <c r="Z72" s="1"/>
       <c r="AL72" s="1"/>
     </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:38" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="1"/>
-      <c r="M73" s="1"/>
-      <c r="N73" s="1"/>
-      <c r="O73" s="1"/>
+      <c r="B73" s="5">
+        <v>2</v>
+      </c>
+      <c r="C73" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="D73" s="80"/>
+      <c r="E73" s="80"/>
+      <c r="F73" s="80"/>
+      <c r="G73" s="80"/>
+      <c r="H73" s="80"/>
+      <c r="I73" s="80"/>
+      <c r="J73" s="80"/>
+      <c r="K73" s="80"/>
+      <c r="L73" s="80"/>
+      <c r="M73" s="81"/>
+      <c r="N73" s="54"/>
+      <c r="O73" s="54"/>
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
@@ -5442,22 +5545,26 @@
       <c r="Z73" s="1"/>
       <c r="AL73" s="1"/>
     </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:38" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
+      <c r="B74" s="6">
+        <v>1</v>
+      </c>
+      <c r="C74" s="79" t="s">
+        <v>86</v>
+      </c>
+      <c r="D74" s="80"/>
+      <c r="E74" s="80"/>
+      <c r="F74" s="80"/>
+      <c r="G74" s="80"/>
+      <c r="H74" s="80"/>
+      <c r="I74" s="80"/>
+      <c r="J74" s="80"/>
+      <c r="K74" s="80"/>
+      <c r="L74" s="80"/>
+      <c r="M74" s="81"/>
+      <c r="N74" s="54"/>
+      <c r="O74" s="54"/>
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
@@ -5471,22 +5578,26 @@
       <c r="Z74" s="1"/>
       <c r="AL74" s="1"/>
     </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:38" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-      <c r="M75" s="1"/>
-      <c r="N75" s="1"/>
-      <c r="O75" s="1"/>
+      <c r="B75" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="D75" s="80"/>
+      <c r="E75" s="80"/>
+      <c r="F75" s="80"/>
+      <c r="G75" s="80"/>
+      <c r="H75" s="80"/>
+      <c r="I75" s="80"/>
+      <c r="J75" s="80"/>
+      <c r="K75" s="80"/>
+      <c r="L75" s="80"/>
+      <c r="M75" s="81"/>
+      <c r="N75" s="54"/>
+      <c r="O75" s="54"/>
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
@@ -5529,10 +5640,12 @@
       <c r="Z76" s="1"/>
       <c r="AL76" s="1"/>
     </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="C77" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -5558,10 +5671,12 @@
       <c r="Z77" s="1"/>
       <c r="AL77" s="1"/>
     </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="C78" s="53" t="s">
+        <v>90</v>
+      </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -5937,13 +6052,216 @@
     </row>
     <row r="91" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1"/>
+      <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
+      <c r="S91" s="1"/>
+      <c r="T91" s="1"/>
+      <c r="U91" s="1"/>
+      <c r="V91" s="1"/>
+      <c r="W91" s="1"/>
+      <c r="X91" s="1"/>
+      <c r="Y91" s="1"/>
+      <c r="Z91" s="1"/>
+      <c r="AL91" s="1"/>
+    </row>
+    <row r="92" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+      <c r="R92" s="1"/>
+      <c r="S92" s="1"/>
+      <c r="T92" s="1"/>
+      <c r="U92" s="1"/>
+      <c r="V92" s="1"/>
+      <c r="W92" s="1"/>
+      <c r="X92" s="1"/>
+      <c r="Y92" s="1"/>
+      <c r="Z92" s="1"/>
+      <c r="AL92" s="1"/>
+    </row>
+    <row r="93" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+      <c r="L93" s="1"/>
+      <c r="M93" s="1"/>
+      <c r="N93" s="1"/>
+      <c r="O93" s="1"/>
+      <c r="P93" s="1"/>
+      <c r="Q93" s="1"/>
+      <c r="R93" s="1"/>
+      <c r="S93" s="1"/>
+      <c r="T93" s="1"/>
+      <c r="U93" s="1"/>
+      <c r="V93" s="1"/>
+      <c r="W93" s="1"/>
+      <c r="X93" s="1"/>
+      <c r="Y93" s="1"/>
+      <c r="Z93" s="1"/>
+      <c r="AL93" s="1"/>
+    </row>
+    <row r="94" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="1"/>
+      <c r="S94" s="1"/>
+      <c r="T94" s="1"/>
+      <c r="U94" s="1"/>
+      <c r="V94" s="1"/>
+      <c r="W94" s="1"/>
+      <c r="X94" s="1"/>
+      <c r="Y94" s="1"/>
+      <c r="Z94" s="1"/>
+      <c r="AL94" s="1"/>
+    </row>
+    <row r="95" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="1"/>
+      <c r="S95" s="1"/>
+      <c r="T95" s="1"/>
+      <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+      <c r="W95" s="1"/>
+      <c r="X95" s="1"/>
+      <c r="Y95" s="1"/>
+      <c r="Z95" s="1"/>
+      <c r="AL95" s="1"/>
+    </row>
+    <row r="96" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
+      <c r="L96" s="1"/>
+      <c r="M96" s="1"/>
+      <c r="N96" s="1"/>
+      <c r="O96" s="1"/>
+      <c r="P96" s="1"/>
+      <c r="Q96" s="1"/>
+      <c r="R96" s="1"/>
+      <c r="S96" s="1"/>
+      <c r="T96" s="1"/>
+      <c r="U96" s="1"/>
+      <c r="V96" s="1"/>
+      <c r="W96" s="1"/>
+      <c r="X96" s="1"/>
+      <c r="Y96" s="1"/>
+      <c r="Z96" s="1"/>
+      <c r="AL96" s="1"/>
+    </row>
+    <row r="97" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1"/>
+      <c r="R97" s="1"/>
+      <c r="S97" s="1"/>
+      <c r="T97" s="1"/>
+      <c r="U97" s="1"/>
+      <c r="V97" s="1"/>
+      <c r="W97" s="1"/>
+      <c r="X97" s="1"/>
+      <c r="Y97" s="1"/>
+      <c r="Z97" s="1"/>
+      <c r="AL97" s="1"/>
+    </row>
+    <row r="98" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A98" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C65:M65"/>
-    <mergeCell ref="C66:M66"/>
-    <mergeCell ref="C67:M67"/>
-    <mergeCell ref="C68:M68"/>
+    <mergeCell ref="C72:M72"/>
+    <mergeCell ref="C73:M73"/>
+    <mergeCell ref="C74:M74"/>
+    <mergeCell ref="C75:M75"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.19" right="0.17" top="0.35" bottom="0.37" header="0.21" footer="0.24"/>

</xml_diff>